<commit_message>
Revised report sections on data scaling and model architecture
</commit_message>
<xml_diff>
--- a/distribucion.xlsx
+++ b/distribucion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesli\OneDrive\Escritorio\IA\IA_imageRecognition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1822d3d40a7589dd/Escritorio/IA/IA_imageRecognition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9D829D-F9B3-42DE-A76F-81697CB71856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{FF9D829D-F9B3-42DE-A76F-81697CB71856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{567F6B4B-9C2C-41BA-B48F-993BCE60C755}"/>
   <bookViews>
-    <workbookView xWindow="10550" yWindow="0" windowWidth="8740" windowHeight="10170" xr2:uid="{E7B1D1B6-3C07-43C7-A73D-EC733EDE4AB9}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{E7B1D1B6-3C07-43C7-A73D-EC733EDE4AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Abra</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>total</t>
-  </si>
-  <si>
-    <t>Quitar</t>
   </si>
 </sst>
 </file>
@@ -109,7 +106,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -450,15 +457,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A2AB3A1-83FF-4F0C-BA57-2E4DACCC533D}">
-  <dimension ref="B1:G12"/>
+  <dimension ref="B1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -468,11 +475,8 @@
       <c r="E1" s="2">
         <v>0.2</v>
       </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -487,12 +491,8 @@
         <f>C2-D2</f>
         <v>80.799999999999955</v>
       </c>
-      <c r="G2">
-        <f>C2-C12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -507,12 +507,8 @@
         <f t="shared" ref="E3:E9" si="1">C3-D3</f>
         <v>80.799999999999955</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G9" si="2">C3-C13</f>
-        <v>404</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -527,12 +523,8 @@
         <f t="shared" si="1"/>
         <v>80.799999999999955</v>
       </c>
-      <c r="G4">
-        <f t="shared" si="2"/>
-        <v>404</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -547,12 +539,8 @@
         <f t="shared" si="1"/>
         <v>80.799999999999955</v>
       </c>
-      <c r="G5">
-        <f t="shared" si="2"/>
-        <v>404</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -567,12 +555,8 @@
         <f t="shared" si="1"/>
         <v>80.799999999999955</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="2"/>
-        <v>404</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -587,12 +571,8 @@
         <f t="shared" si="1"/>
         <v>80.799999999999955</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="2"/>
-        <v>404</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -607,12 +587,8 @@
         <f t="shared" si="1"/>
         <v>80.799999999999955</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="2"/>
-        <v>404</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -627,21 +603,22 @@
         <f t="shared" si="1"/>
         <v>80.799999999999955</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="2"/>
-        <v>404</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C12">
-        <f>MIN(C2:C9)</f>
-        <v>404</v>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <f>SUM(C2:C9)</f>
+        <v>3232</v>
+      </c>
+      <c r="D11" s="1">
+        <f>C11-E11</f>
+        <v>2584</v>
+      </c>
+      <c r="E11" s="1">
+        <f>81*8</f>
+        <v>648</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C12">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>